<commit_message>
alguns acertos na sprint_Backlog
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Planilhas/Sprint_Backlog.xlsx
+++ b/Projeto-Documentacao/Planilhas/Sprint_Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\REGINALDO\Documents\Curso do Romão\Pesquisa-inovacao-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\REGINALDO\Desktop\grupo3-sa\Projeto-Documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C640469-C340-43BE-A1EB-A27F11F06572}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6C8633-87B8-49D0-BC81-3E6DC0BB53D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Descrição</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Realizar Conexão com Arduino UNO.</t>
+  </si>
+  <si>
+    <t>Realizar</t>
   </si>
 </sst>
 </file>
@@ -247,17 +250,20 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -265,19 +271,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +608,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,422 +622,455 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="8">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>4</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="8">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="8">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>3</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="7" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="8">
         <v>5</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="8">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="3" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="3" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>6</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="6">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>2</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="7" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="8">
         <v>7</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="8">
         <v>2</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="3" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="3" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="10">
         <v>8</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="10">
         <v>2</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="10"/>
+      <c r="E32" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="10" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="10"/>
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="10" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="10"/>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="10" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="C32:C35"/>
@@ -1044,15 +1080,12 @@
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="C25:C28"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>